<commit_message>
updated cookbook test for resource types
</commit_message>
<xml_diff>
--- a/doc/user-guide/cookbook/resource/resource-type.xlsx
+++ b/doc/user-guide/cookbook/resource/resource-type.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\frepple-community-4.2\doc\user-guide\cookbook\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\frepple-community\doc\user-guide\cookbook\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16500" windowHeight="7545" tabRatio="946" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16500" windowHeight="7545" tabRatio="946" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="buffer" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7132" uniqueCount="3561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7143" uniqueCount="3565">
   <si>
     <t>name</t>
   </si>
@@ -10715,6 +10715,18 @@
   </si>
   <si>
     <t>minimum shipment</t>
+  </si>
+  <si>
+    <t>Resource D</t>
+  </si>
+  <si>
+    <t>buckets_month</t>
+  </si>
+  <si>
+    <t>Resource E</t>
+  </si>
+  <si>
+    <t>infinite</t>
   </si>
 </sst>
 </file>
@@ -11273,16 +11285,16 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.9296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11342,6 +11354,31 @@
         <v>1375</v>
       </c>
       <c r="E4" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>3561</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3562</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1369</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>3563</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3564</v>
+      </c>
+      <c r="E6" t="s">
         <v>1367</v>
       </c>
     </row>
@@ -60457,7 +60494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -60761,10 +60798,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -60815,6 +60852,28 @@
         <v>1364</v>
       </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3561</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3563</v>
+      </c>
+      <c r="C6">
         <v>1</v>
       </c>
     </row>

</xml_diff>